<commit_message>
Adding comparison data listed in the paper
</commit_message>
<xml_diff>
--- a/Leon_Contribution_102424.xlsx
+++ b/Leon_Contribution_102424.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Github-Codes\ULTERA-contribute-Leon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987D1796-1EFD-46C9-91EF-749132CF0F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055E669C-3400-45AD-BE6C-CBC764BC9C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="191">
   <si>
     <t>Name:</t>
   </si>
@@ -724,6 +724,102 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2021.159190</t>
+  </si>
+  <si>
+    <t>Ti30.3 Zr30.3 Nb30.3 Ta3.0 Al6.1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ti32.3 Zr32.3 Nb32.3 Ta3.1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCC+Al3Zr5</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ti40 Zr20 Nb20 Hf20</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCC</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ti38.6 Zr19.2 Nb19.2 Hf19.2 V3.8</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ti37.0 Zr18.5 Nb18.5 Hf18.5 V7.5</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ti35.6 Zr17.9 Nb17.9 Hf17.9 V10.7</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ti34.6 Zr17.2 Nb17.2 Hf17.2 V13.8</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ti33.3 Zr16.7 Nb16.7 Hf16.7 V16.7</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ti20 Zr20 Nb20 Mo20 V20</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ti27.20 Zr18.2 Nb18.2 Mo18.20 V18.20</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ti33.20 Zr16.7 Nb16.7 Mo16.70 V16.70</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Al10 Nb20 Ti20 V40 Zr10</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Al9.1 Nb18.2 Ti18.2 V26.3 Zr18.2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Al9.1 Nb9.1 Ti18.2 V36.4 Zr27.2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Al11.1 Nb22.2 Ti22.2 V44.5 Zr11.1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Al10. Nb20.0 Ti20.0 V40.0 Zr10.0</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hf20 Nb20 Ta20 Ti20 Zr20</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Al5.5 Hf18.9 Nb18.9 Ta18.9 Ti18.9 Zr18.9</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Al9 Hf18.2 Nb18.2 Ta18.2 Ti18.2 Zr18.2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Al13.0 Hf17.4 Nb17.4 Ta17.4 Ti17.4 Zr17.4</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Al16.7 Hf16.7 Nb16.7 Ta16.7 Ti16.6 Zr16.6</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hf12.5 Mo12.5 Nb25 Ti25 Zr25</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1464,32 +1560,8 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1542,8 +1614,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1828,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.45"/>
@@ -1865,19 +1961,19 @@
       <c r="B2" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="58"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="50"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1">
@@ -1887,17 +1983,17 @@
       <c r="B3" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="60"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1">
@@ -1915,43 +2011,43 @@
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="54" t="s">
+      <c r="F5" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="54" t="s">
+      <c r="G5" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="54" t="s">
+      <c r="J5" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="54" t="s">
+      <c r="K5" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="54" t="s">
+      <c r="L5" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="54" t="s">
+      <c r="M5" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="54" t="s">
+      <c r="N5" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="48" t="s">
+      <c r="O5" s="67" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1962,19 +2058,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="49"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="68"/>
     </row>
     <row r="7" spans="1:20" ht="17.149999999999999" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -2019,7 +2115,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="50"/>
+      <c r="O7" s="69"/>
       <c r="P7" s="30" t="s">
         <v>40</v>
       </c>
@@ -2032,35 +2128,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="68" t="s">
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="71" t="s">
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="72"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="51" t="s">
+      <c r="P8" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="52"/>
-      <c r="S8" s="52"/>
-      <c r="T8" s="53"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="72"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1">
       <c r="A9" s="2" t="s">
@@ -2325,7 +2421,7 @@
         <v>81</v>
       </c>
       <c r="E15" s="19"/>
-      <c r="F15" s="74" t="s">
+      <c r="F15" s="48" t="s">
         <v>145</v>
       </c>
       <c r="G15" s="40" t="s">
@@ -2403,7 +2499,7 @@
         <v>81</v>
       </c>
       <c r="E17" s="19"/>
-      <c r="F17" s="74" t="s">
+      <c r="F17" s="48" t="s">
         <v>145</v>
       </c>
       <c r="G17" s="40" t="s">
@@ -2481,7 +2577,7 @@
         <v>81</v>
       </c>
       <c r="E19" s="19"/>
-      <c r="F19" s="74" t="s">
+      <c r="F19" s="48" t="s">
         <v>145</v>
       </c>
       <c r="G19" s="40" t="s">
@@ -2559,7 +2655,7 @@
         <v>84</v>
       </c>
       <c r="E21" s="19"/>
-      <c r="F21" s="74" t="s">
+      <c r="F21" s="48" t="s">
         <v>145</v>
       </c>
       <c r="G21" s="40" t="s">
@@ -2597,7 +2693,7 @@
       <c r="E22" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="74" t="s">
+      <c r="F22" s="48" t="s">
         <v>145</v>
       </c>
       <c r="G22" s="40" t="s">
@@ -2635,7 +2731,7 @@
       <c r="E23" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="74" t="s">
+      <c r="F23" s="48" t="s">
         <v>145</v>
       </c>
       <c r="G23" s="40" t="s">
@@ -2895,7 +2991,7 @@
         <v>81</v>
       </c>
       <c r="E30" s="19"/>
-      <c r="F30" s="74" t="s">
+      <c r="F30" s="48" t="s">
         <v>145</v>
       </c>
       <c r="G30" s="40" t="s">
@@ -2933,7 +3029,7 @@
         <v>81</v>
       </c>
       <c r="E31" s="19"/>
-      <c r="F31" s="74" t="s">
+      <c r="F31" s="48" t="s">
         <v>145</v>
       </c>
       <c r="G31" s="40" t="s">
@@ -3047,7 +3143,7 @@
         <v>81</v>
       </c>
       <c r="E34" s="19"/>
-      <c r="F34" s="74" t="s">
+      <c r="F34" s="48" t="s">
         <v>145</v>
       </c>
       <c r="G34" s="40" t="s">
@@ -3085,7 +3181,7 @@
         <v>81</v>
       </c>
       <c r="E35" s="19"/>
-      <c r="F35" s="74" t="s">
+      <c r="F35" s="48" t="s">
         <v>145</v>
       </c>
       <c r="G35" s="40" t="s">
@@ -6740,965 +6836,2020 @@
         <v>166</v>
       </c>
     </row>
-    <row r="134" spans="1:14">
+    <row r="134" spans="1:14" ht="16.3">
       <c r="A134" s="35"/>
-      <c r="B134" s="19"/>
-      <c r="C134" s="32"/>
+      <c r="B134" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C134" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="D134" s="32"/>
       <c r="E134" s="19"/>
-      <c r="F134" s="32"/>
-      <c r="G134" s="32"/>
+      <c r="F134" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G134" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H134" s="32"/>
-      <c r="I134" s="34"/>
-      <c r="J134" s="31"/>
-      <c r="K134" s="31"/>
-      <c r="L134" s="19"/>
-      <c r="M134" s="19"/>
-      <c r="N134" s="19"/>
-    </row>
-    <row r="135" spans="1:14">
+      <c r="I134" s="34">
+        <v>298</v>
+      </c>
+      <c r="J134" s="31">
+        <v>1022000000</v>
+      </c>
+      <c r="K134" s="31">
+        <v>51000000</v>
+      </c>
+      <c r="L134" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M134" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N134" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" ht="16.3">
       <c r="A135" s="35"/>
-      <c r="B135" s="19"/>
-      <c r="C135" s="32"/>
+      <c r="B135" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C135" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="D135" s="32"/>
       <c r="E135" s="19"/>
-      <c r="F135" s="32"/>
-      <c r="G135" s="32"/>
+      <c r="F135" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G135" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H135" s="32"/>
-      <c r="I135" s="34"/>
-      <c r="J135" s="31"/>
+      <c r="I135" s="34">
+        <v>298</v>
+      </c>
+      <c r="J135" s="31">
+        <v>6.74</v>
+      </c>
       <c r="K135" s="31"/>
-      <c r="L135" s="19"/>
-      <c r="M135" s="19"/>
-      <c r="N135" s="19"/>
-    </row>
-    <row r="136" spans="1:14">
-      <c r="A136" s="35"/>
-      <c r="B136" s="19"/>
-      <c r="C136" s="32"/>
-      <c r="D136" s="32"/>
-      <c r="E136" s="19"/>
-      <c r="F136" s="32"/>
-      <c r="G136" s="32"/>
-      <c r="H136" s="32"/>
-      <c r="I136" s="34"/>
-      <c r="J136" s="31"/>
-      <c r="K136" s="31"/>
-      <c r="L136" s="19"/>
-      <c r="M136" s="19"/>
-      <c r="N136" s="19"/>
-    </row>
-    <row r="137" spans="1:14">
+      <c r="L135" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M135" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N135" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" ht="16.3">
+      <c r="B136" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C136" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="F136" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G136" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I136" s="34">
+        <v>298</v>
+      </c>
+      <c r="J136" s="31">
+        <v>1037000000</v>
+      </c>
+      <c r="K136" s="31">
+        <v>178000000</v>
+      </c>
+      <c r="L136" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M136" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N136" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" ht="16.3">
       <c r="A137" s="35"/>
-      <c r="B137" s="19"/>
-      <c r="C137" s="32"/>
+      <c r="B137" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C137" s="32" t="s">
+        <v>169</v>
+      </c>
       <c r="D137" s="32"/>
       <c r="E137" s="19"/>
-      <c r="F137" s="32"/>
-      <c r="G137" s="32"/>
+      <c r="F137" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G137" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H137" s="32"/>
-      <c r="I137" s="34"/>
-      <c r="J137" s="31"/>
+      <c r="I137" s="34">
+        <v>298</v>
+      </c>
+      <c r="J137" s="31">
+        <v>6</v>
+      </c>
       <c r="K137" s="31"/>
-      <c r="L137" s="19"/>
-      <c r="M137" s="19"/>
-      <c r="N137" s="19"/>
-    </row>
-    <row r="138" spans="1:14">
+      <c r="L137" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M137" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N137" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" ht="16.3">
       <c r="A138" s="35"/>
-      <c r="B138" s="19"/>
-      <c r="C138" s="32"/>
+      <c r="B138" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C138" s="32" t="s">
+        <v>169</v>
+      </c>
       <c r="D138" s="32"/>
       <c r="E138" s="19"/>
-      <c r="F138" s="32"/>
-      <c r="G138" s="32"/>
+      <c r="F138" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G138" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H138" s="32"/>
-      <c r="I138" s="34"/>
-      <c r="J138" s="31"/>
+      <c r="I138" s="34">
+        <v>298</v>
+      </c>
+      <c r="J138" s="31">
+        <v>6.11</v>
+      </c>
       <c r="K138" s="31"/>
-      <c r="L138" s="19"/>
-      <c r="M138" s="19"/>
-      <c r="N138" s="19"/>
-    </row>
-    <row r="139" spans="1:14">
+      <c r="L138" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M138" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N138" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" ht="16.3">
       <c r="A139" s="35"/>
-      <c r="B139" s="19"/>
-      <c r="C139" s="32"/>
+      <c r="B139" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C139" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="D139" s="32"/>
       <c r="E139" s="19"/>
-      <c r="F139" s="32"/>
-      <c r="G139" s="32"/>
+      <c r="F139" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G139" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H139" s="32"/>
-      <c r="I139" s="34"/>
-      <c r="J139" s="31"/>
-      <c r="K139" s="31"/>
-      <c r="L139" s="19"/>
-      <c r="M139" s="19"/>
-      <c r="N139" s="19"/>
-    </row>
-    <row r="140" spans="1:14">
+      <c r="I139" s="34">
+        <v>298</v>
+      </c>
+      <c r="J139" s="31">
+        <v>1022000000</v>
+      </c>
+      <c r="K139" s="31">
+        <v>51000000</v>
+      </c>
+      <c r="L139" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M139" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N139" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" ht="16.3">
       <c r="A140" s="35"/>
-      <c r="B140" s="19"/>
-      <c r="C140" s="32"/>
+      <c r="B140" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C140" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="D140" s="32"/>
       <c r="E140" s="19"/>
-      <c r="F140" s="32"/>
-      <c r="G140" s="32"/>
+      <c r="F140" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G140" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H140" s="32"/>
-      <c r="I140" s="34"/>
-      <c r="J140" s="31"/>
+      <c r="I140" s="34">
+        <v>298</v>
+      </c>
+      <c r="J140" s="31">
+        <v>6.74</v>
+      </c>
       <c r="K140" s="31"/>
-      <c r="L140" s="19"/>
-      <c r="M140" s="19"/>
-      <c r="N140" s="19"/>
-    </row>
-    <row r="141" spans="1:14">
+      <c r="L140" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M140" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N140" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" ht="16.3">
       <c r="A141" s="35"/>
-      <c r="B141" s="19"/>
-      <c r="C141" s="32"/>
+      <c r="B141" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C141" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D141" s="32"/>
       <c r="E141" s="19"/>
-      <c r="F141" s="32"/>
-      <c r="G141" s="32"/>
+      <c r="F141" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G141" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H141" s="32"/>
-      <c r="I141" s="34"/>
-      <c r="J141" s="31"/>
+      <c r="I141" s="34">
+        <v>298</v>
+      </c>
+      <c r="J141" s="31">
+        <v>613000000</v>
+      </c>
       <c r="K141" s="31"/>
-      <c r="L141" s="19"/>
-      <c r="M141" s="19"/>
-      <c r="N141" s="19"/>
-    </row>
-    <row r="142" spans="1:14">
+      <c r="L141" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M141" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N141" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" ht="16.3">
       <c r="A142" s="35"/>
-      <c r="B142" s="19"/>
-      <c r="C142" s="32"/>
+      <c r="B142" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C142" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="D142" s="32"/>
       <c r="E142" s="19"/>
-      <c r="F142" s="32"/>
-      <c r="G142" s="32"/>
+      <c r="F142" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G142" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H142" s="32"/>
-      <c r="I142" s="34"/>
-      <c r="J142" s="31"/>
+      <c r="I142" s="34">
+        <v>298</v>
+      </c>
+      <c r="J142" s="31">
+        <v>7.7</v>
+      </c>
       <c r="K142" s="31"/>
-      <c r="L142" s="19"/>
-      <c r="M142" s="19"/>
-      <c r="N142" s="19"/>
-    </row>
-    <row r="143" spans="1:14">
+      <c r="L142" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M142" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N142" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" ht="16.3">
       <c r="A143" s="35"/>
-      <c r="B143" s="19"/>
-      <c r="C143" s="32"/>
+      <c r="B143" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C143" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D143" s="32"/>
       <c r="E143" s="19"/>
-      <c r="F143" s="32"/>
-      <c r="G143" s="32"/>
+      <c r="F143" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G143" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H143" s="32"/>
-      <c r="I143" s="34"/>
-      <c r="J143" s="31"/>
+      <c r="I143" s="34">
+        <v>298</v>
+      </c>
+      <c r="J143" s="31">
+        <v>709000000</v>
+      </c>
       <c r="K143" s="31"/>
-      <c r="L143" s="19"/>
-      <c r="M143" s="19"/>
-      <c r="N143" s="19"/>
-    </row>
-    <row r="144" spans="1:14">
+      <c r="L143" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M143" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N143" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" ht="16.3">
       <c r="A144" s="35"/>
-      <c r="B144" s="19"/>
-      <c r="C144" s="32"/>
+      <c r="B144" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C144" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="D144" s="32"/>
       <c r="E144" s="19"/>
-      <c r="F144" s="32"/>
-      <c r="G144" s="32"/>
+      <c r="F144" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G144" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H144" s="32"/>
-      <c r="I144" s="34"/>
-      <c r="J144" s="31"/>
+      <c r="I144" s="34">
+        <v>298</v>
+      </c>
+      <c r="J144" s="31">
+        <v>7.66</v>
+      </c>
       <c r="K144" s="31"/>
-      <c r="L144" s="19"/>
-      <c r="M144" s="19"/>
-      <c r="N144" s="19"/>
-    </row>
-    <row r="145" spans="1:14">
+      <c r="L144" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M144" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N144" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" ht="16.3">
       <c r="A145" s="35"/>
-      <c r="B145" s="19"/>
-      <c r="C145" s="32"/>
+      <c r="B145" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C145" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D145" s="32"/>
       <c r="E145" s="19"/>
-      <c r="F145" s="32"/>
-      <c r="G145" s="32"/>
+      <c r="F145" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G145" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H145" s="32"/>
-      <c r="I145" s="34"/>
-      <c r="J145" s="31"/>
+      <c r="I145" s="34">
+        <v>298</v>
+      </c>
+      <c r="J145" s="31">
+        <v>829000000</v>
+      </c>
       <c r="K145" s="31"/>
-      <c r="L145" s="19"/>
-      <c r="M145" s="19"/>
-      <c r="N145" s="19"/>
-    </row>
-    <row r="146" spans="1:14">
+      <c r="L145" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M145" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N145" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" ht="16.3">
       <c r="A146" s="35"/>
-      <c r="B146" s="19"/>
-      <c r="C146" s="32"/>
+      <c r="B146" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C146" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="D146" s="32"/>
       <c r="E146" s="19"/>
-      <c r="F146" s="32"/>
-      <c r="G146" s="32"/>
+      <c r="F146" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G146" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H146" s="32"/>
-      <c r="I146" s="34"/>
-      <c r="J146" s="31"/>
+      <c r="I146" s="34">
+        <v>298</v>
+      </c>
+      <c r="J146" s="31">
+        <v>7.63</v>
+      </c>
       <c r="K146" s="31"/>
-      <c r="L146" s="19"/>
-      <c r="M146" s="19"/>
-      <c r="N146" s="19"/>
-    </row>
-    <row r="147" spans="1:14">
+      <c r="L146" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M146" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N146" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" ht="16.3">
       <c r="A147" s="35"/>
-      <c r="B147" s="19"/>
-      <c r="C147" s="32"/>
+      <c r="B147" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C147" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D147" s="32"/>
       <c r="E147" s="19"/>
-      <c r="F147" s="32"/>
-      <c r="G147" s="32"/>
+      <c r="F147" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G147" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H147" s="32"/>
-      <c r="I147" s="34"/>
-      <c r="J147" s="31"/>
+      <c r="I147" s="34">
+        <v>298</v>
+      </c>
+      <c r="J147" s="31">
+        <v>859000000</v>
+      </c>
       <c r="K147" s="31"/>
-      <c r="L147" s="19"/>
-      <c r="M147" s="19"/>
-      <c r="N147" s="19"/>
-    </row>
-    <row r="148" spans="1:14">
+      <c r="L147" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M147" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N147" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" ht="16.3">
       <c r="A148" s="35"/>
-      <c r="B148" s="19"/>
-      <c r="C148" s="32"/>
+      <c r="B148" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C148" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="D148" s="32"/>
       <c r="E148" s="19"/>
-      <c r="F148" s="32"/>
-      <c r="G148" s="32"/>
+      <c r="F148" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G148" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H148" s="32"/>
-      <c r="I148" s="34"/>
-      <c r="J148" s="31"/>
+      <c r="I148" s="34">
+        <v>298</v>
+      </c>
+      <c r="J148" s="31">
+        <v>7.59</v>
+      </c>
       <c r="K148" s="31"/>
-      <c r="L148" s="19"/>
-      <c r="M148" s="19"/>
-      <c r="N148" s="19"/>
-    </row>
-    <row r="149" spans="1:14">
+      <c r="L148" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M148" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N148" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" ht="16.3">
       <c r="A149" s="35"/>
-      <c r="B149" s="19"/>
-      <c r="C149" s="32"/>
+      <c r="B149" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C149" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D149" s="32"/>
       <c r="E149" s="19"/>
-      <c r="F149" s="32"/>
-      <c r="G149" s="32"/>
+      <c r="F149" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G149" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H149" s="32"/>
-      <c r="I149" s="34"/>
-      <c r="J149" s="31"/>
+      <c r="I149" s="34">
+        <v>298</v>
+      </c>
+      <c r="J149" s="31">
+        <v>946000000</v>
+      </c>
       <c r="K149" s="31"/>
-      <c r="L149" s="19"/>
-      <c r="M149" s="19"/>
-      <c r="N149" s="19"/>
-    </row>
-    <row r="150" spans="1:14">
+      <c r="L149" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M149" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N149" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" ht="16.3">
       <c r="A150" s="35"/>
-      <c r="B150" s="19"/>
-      <c r="C150" s="32"/>
+      <c r="B150" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C150" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="D150" s="32"/>
       <c r="E150" s="19"/>
-      <c r="F150" s="32"/>
-      <c r="G150" s="32"/>
+      <c r="F150" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G150" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H150" s="32"/>
-      <c r="I150" s="34"/>
-      <c r="J150" s="31"/>
+      <c r="I150" s="34">
+        <v>298</v>
+      </c>
+      <c r="J150" s="31">
+        <v>7.54</v>
+      </c>
       <c r="K150" s="31"/>
-      <c r="L150" s="19"/>
-      <c r="M150" s="19"/>
-      <c r="N150" s="19"/>
-    </row>
-    <row r="151" spans="1:14">
+      <c r="L150" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M150" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N150" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" ht="16.3">
       <c r="A151" s="35"/>
-      <c r="B151" s="19"/>
-      <c r="C151" s="32"/>
+      <c r="B151" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C151" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D151" s="32"/>
       <c r="E151" s="19"/>
-      <c r="F151" s="32"/>
-      <c r="G151" s="32"/>
+      <c r="F151" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G151" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H151" s="32"/>
-      <c r="I151" s="34"/>
-      <c r="J151" s="31"/>
+      <c r="I151" s="34">
+        <v>298</v>
+      </c>
+      <c r="J151" s="31">
+        <v>1007000000</v>
+      </c>
       <c r="K151" s="31"/>
-      <c r="L151" s="19"/>
-      <c r="M151" s="19"/>
-      <c r="N151" s="19"/>
-    </row>
-    <row r="152" spans="1:14">
+      <c r="L151" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M151" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N151" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="16.3">
       <c r="A152" s="35"/>
-      <c r="B152" s="19"/>
-      <c r="C152" s="32"/>
+      <c r="B152" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C152" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="D152" s="32"/>
       <c r="E152" s="19"/>
-      <c r="F152" s="32"/>
-      <c r="G152" s="32"/>
+      <c r="F152" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G152" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H152" s="32"/>
-      <c r="I152" s="34"/>
-      <c r="J152" s="31"/>
+      <c r="I152" s="34">
+        <v>298</v>
+      </c>
+      <c r="J152" s="31">
+        <v>7510</v>
+      </c>
       <c r="K152" s="31"/>
-      <c r="L152" s="19"/>
-      <c r="M152" s="19"/>
-      <c r="N152" s="19"/>
-    </row>
-    <row r="153" spans="1:14">
-      <c r="A153" s="35"/>
-      <c r="B153" s="19"/>
-      <c r="C153" s="32"/>
-      <c r="D153" s="32"/>
-      <c r="E153" s="19"/>
-      <c r="F153" s="32"/>
-      <c r="G153" s="32"/>
-      <c r="H153" s="32"/>
-      <c r="I153" s="34"/>
-      <c r="J153" s="31"/>
+      <c r="L152" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M152" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N152" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" ht="16.3">
+      <c r="B153" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C153" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F153" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G153" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I153" s="34">
+        <v>298</v>
+      </c>
+      <c r="J153" s="31">
+        <v>2222000000</v>
+      </c>
       <c r="K153" s="31"/>
-      <c r="L153" s="19"/>
-      <c r="M153" s="19"/>
-      <c r="N153" s="19"/>
-    </row>
-    <row r="154" spans="1:14">
+      <c r="L153" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M153" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N153" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" ht="16.3">
       <c r="A154" s="35"/>
-      <c r="B154" s="19"/>
-      <c r="C154" s="32"/>
+      <c r="B154" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C154" s="32" t="s">
+        <v>103</v>
+      </c>
       <c r="D154" s="32"/>
       <c r="E154" s="19"/>
-      <c r="F154" s="32"/>
-      <c r="G154" s="32"/>
+      <c r="F154" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G154" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H154" s="32"/>
-      <c r="I154" s="34"/>
-      <c r="J154" s="31"/>
+      <c r="I154" s="34">
+        <v>298</v>
+      </c>
+      <c r="J154" s="31">
+        <v>20.5</v>
+      </c>
       <c r="K154" s="31"/>
-      <c r="L154" s="19"/>
-      <c r="M154" s="19"/>
-      <c r="N154" s="19"/>
-    </row>
-    <row r="155" spans="1:14">
+      <c r="L154" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M154" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N154" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" ht="16.3">
       <c r="A155" s="35"/>
-      <c r="B155" s="19"/>
-      <c r="C155" s="32"/>
+      <c r="B155" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C155" s="32" t="s">
+        <v>103</v>
+      </c>
       <c r="D155" s="32"/>
       <c r="E155" s="19"/>
-      <c r="F155" s="32"/>
-      <c r="G155" s="32"/>
+      <c r="F155" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G155" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H155" s="32"/>
-      <c r="I155" s="34"/>
-      <c r="J155" s="31"/>
+      <c r="I155" s="34">
+        <v>298</v>
+      </c>
+      <c r="J155" s="31">
+        <v>7.13</v>
+      </c>
       <c r="K155" s="31"/>
-      <c r="L155" s="19"/>
-      <c r="M155" s="19"/>
-      <c r="N155" s="19"/>
-    </row>
-    <row r="156" spans="1:14">
-      <c r="A156" s="35"/>
-      <c r="B156" s="19"/>
-      <c r="C156" s="32"/>
-      <c r="D156" s="32"/>
-      <c r="E156" s="19"/>
-      <c r="F156" s="32"/>
-      <c r="G156" s="32"/>
-      <c r="H156" s="32"/>
-      <c r="I156" s="34"/>
-      <c r="J156" s="31"/>
+      <c r="L155" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M155" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N155" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" ht="16.3">
+      <c r="B156" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C156" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F156" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G156" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I156" s="34">
+        <v>298</v>
+      </c>
+      <c r="J156" s="31">
+        <v>1691000000</v>
+      </c>
       <c r="K156" s="31"/>
-      <c r="L156" s="19"/>
-      <c r="M156" s="19"/>
-      <c r="N156" s="19"/>
-    </row>
-    <row r="157" spans="1:14">
+      <c r="L156" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M156" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N156" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" ht="16.3">
       <c r="A157" s="35"/>
-      <c r="B157" s="19"/>
-      <c r="C157" s="32"/>
+      <c r="B157" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C157" s="32" t="s">
+        <v>103</v>
+      </c>
       <c r="D157" s="32"/>
       <c r="E157" s="19"/>
-      <c r="F157" s="32"/>
-      <c r="G157" s="32"/>
+      <c r="F157" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G157" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H157" s="32"/>
-      <c r="I157" s="34"/>
-      <c r="J157" s="31"/>
+      <c r="I157" s="34">
+        <v>298</v>
+      </c>
+      <c r="J157" s="31">
+        <v>23.2</v>
+      </c>
       <c r="K157" s="31"/>
-      <c r="L157" s="19"/>
-      <c r="M157" s="19"/>
-      <c r="N157" s="19"/>
-    </row>
-    <row r="158" spans="1:14">
+      <c r="L157" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M157" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N157" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" ht="16.3">
       <c r="A158" s="35"/>
-      <c r="B158" s="19"/>
-      <c r="C158" s="32"/>
+      <c r="B158" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C158" s="32" t="s">
+        <v>103</v>
+      </c>
       <c r="D158" s="32"/>
       <c r="E158" s="19"/>
-      <c r="F158" s="32"/>
-      <c r="G158" s="32"/>
+      <c r="F158" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G158" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H158" s="32"/>
-      <c r="I158" s="34"/>
-      <c r="J158" s="31"/>
+      <c r="I158" s="34">
+        <v>298</v>
+      </c>
+      <c r="J158" s="31">
+        <v>6890</v>
+      </c>
       <c r="K158" s="31"/>
-      <c r="L158" s="19"/>
-      <c r="M158" s="19"/>
-      <c r="N158" s="19"/>
-    </row>
-    <row r="159" spans="1:14">
-      <c r="A159" s="35"/>
-      <c r="B159" s="19"/>
-      <c r="C159" s="32"/>
-      <c r="D159" s="32"/>
-      <c r="E159" s="19"/>
-      <c r="F159" s="32"/>
-      <c r="G159" s="32"/>
-      <c r="H159" s="32"/>
-      <c r="I159" s="34"/>
-      <c r="J159" s="31"/>
+      <c r="L158" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M158" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N158" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" ht="16.3">
+      <c r="B159" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C159" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F159" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G159" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I159" s="34">
+        <v>298</v>
+      </c>
+      <c r="J159" s="31">
+        <v>1588000000</v>
+      </c>
       <c r="K159" s="31"/>
-      <c r="L159" s="19"/>
-      <c r="M159" s="19"/>
-      <c r="N159" s="19"/>
-    </row>
-    <row r="160" spans="1:14">
+      <c r="L159" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M159" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N159" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" ht="16.3">
       <c r="A160" s="35"/>
-      <c r="B160" s="19"/>
-      <c r="C160" s="32"/>
+      <c r="B160" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C160" s="32" t="s">
+        <v>103</v>
+      </c>
       <c r="D160" s="32"/>
       <c r="E160" s="19"/>
-      <c r="F160" s="32"/>
-      <c r="G160" s="32"/>
+      <c r="F160" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G160" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H160" s="32"/>
-      <c r="I160" s="34"/>
-      <c r="J160" s="31"/>
+      <c r="I160" s="34">
+        <v>298</v>
+      </c>
+      <c r="J160" s="31">
+        <v>25.8</v>
+      </c>
       <c r="K160" s="31"/>
-      <c r="L160" s="19"/>
-      <c r="M160" s="19"/>
-      <c r="N160" s="19"/>
-    </row>
-    <row r="161" spans="1:14">
+      <c r="L160" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M160" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N160" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="16.3">
       <c r="A161" s="35"/>
-      <c r="B161" s="19"/>
-      <c r="C161" s="32"/>
+      <c r="B161" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C161" s="32" t="s">
+        <v>103</v>
+      </c>
       <c r="D161" s="32"/>
       <c r="E161" s="19"/>
-      <c r="F161" s="32"/>
-      <c r="G161" s="32"/>
+      <c r="F161" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G161" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H161" s="32"/>
-      <c r="I161" s="34"/>
-      <c r="J161" s="31"/>
+      <c r="I161" s="34">
+        <v>298</v>
+      </c>
+      <c r="J161" s="31">
+        <v>2.69</v>
+      </c>
       <c r="K161" s="31"/>
-      <c r="L161" s="19"/>
-      <c r="M161" s="19"/>
-      <c r="N161" s="19"/>
-    </row>
-    <row r="162" spans="1:14">
-      <c r="A162" s="35"/>
-      <c r="B162" s="19"/>
-      <c r="C162" s="32"/>
-      <c r="D162" s="32"/>
-      <c r="E162" s="19"/>
-      <c r="F162" s="32"/>
-      <c r="G162" s="32"/>
-      <c r="H162" s="32"/>
-      <c r="I162" s="34"/>
-      <c r="J162" s="31"/>
-      <c r="K162" s="31"/>
-      <c r="L162" s="19"/>
-      <c r="M162" s="19"/>
-      <c r="N162" s="19"/>
-    </row>
-    <row r="163" spans="1:14">
+      <c r="L161" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M161" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N161" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" ht="16.3">
+      <c r="B162" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C162" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F162" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G162" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I162" s="34">
+        <v>298</v>
+      </c>
+      <c r="J162" s="31">
+        <v>1390000000</v>
+      </c>
+      <c r="K162" s="31">
+        <v>11000000</v>
+      </c>
+      <c r="L162" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M162" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N162" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" ht="16.3">
       <c r="A163" s="35"/>
-      <c r="B163" s="19"/>
-      <c r="C163" s="32"/>
+      <c r="B163" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C163" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="D163" s="32"/>
       <c r="E163" s="19"/>
-      <c r="F163" s="32"/>
-      <c r="G163" s="32"/>
+      <c r="F163" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G163" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H163" s="32"/>
-      <c r="I163" s="34"/>
-      <c r="J163" s="31"/>
+      <c r="I163" s="34">
+        <v>298</v>
+      </c>
+      <c r="J163" s="31">
+        <v>16.899999999999999</v>
+      </c>
       <c r="K163" s="31"/>
-      <c r="L163" s="19"/>
-      <c r="M163" s="19"/>
-      <c r="N163" s="19"/>
-    </row>
-    <row r="164" spans="1:14">
+      <c r="L163" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M163" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N163" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" ht="16.3">
       <c r="A164" s="35"/>
-      <c r="B164" s="19"/>
-      <c r="C164" s="32"/>
+      <c r="B164" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C164" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="D164" s="32"/>
       <c r="E164" s="19"/>
-      <c r="F164" s="32"/>
-      <c r="G164" s="32"/>
+      <c r="F164" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G164" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H164" s="32"/>
-      <c r="I164" s="34"/>
-      <c r="J164" s="31"/>
+      <c r="I164" s="34">
+        <v>298</v>
+      </c>
+      <c r="J164" s="31">
+        <v>6.06</v>
+      </c>
       <c r="K164" s="31"/>
-      <c r="L164" s="19"/>
-      <c r="M164" s="19"/>
-      <c r="N164" s="19"/>
-    </row>
-    <row r="165" spans="1:14">
-      <c r="A165" s="35"/>
-      <c r="B165" s="19"/>
-      <c r="C165" s="32"/>
-      <c r="D165" s="32"/>
-      <c r="E165" s="19"/>
-      <c r="F165" s="32"/>
-      <c r="G165" s="32"/>
-      <c r="H165" s="32"/>
-      <c r="I165" s="34"/>
-      <c r="J165" s="31"/>
-      <c r="K165" s="31"/>
-      <c r="L165" s="19"/>
-      <c r="M165" s="19"/>
-      <c r="N165" s="19"/>
-    </row>
-    <row r="166" spans="1:14">
+      <c r="L164" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M164" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N164" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" ht="16.3">
+      <c r="B165" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C165" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F165" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G165" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I165" s="34">
+        <v>298</v>
+      </c>
+      <c r="J165" s="31">
+        <v>1028000000</v>
+      </c>
+      <c r="K165" s="31">
+        <v>25000000</v>
+      </c>
+      <c r="L165" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M165" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N165" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" ht="16.3">
       <c r="A166" s="35"/>
-      <c r="B166" s="19"/>
-      <c r="C166" s="32"/>
+      <c r="B166" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C166" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="D166" s="32"/>
       <c r="E166" s="19"/>
-      <c r="F166" s="32"/>
-      <c r="G166" s="32"/>
+      <c r="F166" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G166" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H166" s="32"/>
-      <c r="I166" s="34"/>
-      <c r="J166" s="31"/>
+      <c r="I166" s="34">
+        <v>298</v>
+      </c>
+      <c r="J166" s="31">
+        <v>9.3000000000000007</v>
+      </c>
       <c r="K166" s="31"/>
-      <c r="L166" s="19"/>
-      <c r="M166" s="19"/>
-      <c r="N166" s="19"/>
-    </row>
-    <row r="167" spans="1:14">
+      <c r="L166" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M166" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N166" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" ht="16.3">
       <c r="A167" s="35"/>
-      <c r="B167" s="19"/>
-      <c r="C167" s="32"/>
+      <c r="B167" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C167" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="D167" s="32"/>
       <c r="E167" s="19"/>
-      <c r="F167" s="32"/>
-      <c r="G167" s="32"/>
+      <c r="F167" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G167" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H167" s="32"/>
-      <c r="I167" s="34"/>
-      <c r="J167" s="31"/>
+      <c r="I167" s="34">
+        <v>298</v>
+      </c>
+      <c r="J167" s="31">
+        <v>6100</v>
+      </c>
       <c r="K167" s="31"/>
-      <c r="L167" s="19"/>
-      <c r="M167" s="19"/>
-      <c r="N167" s="19"/>
-    </row>
-    <row r="168" spans="1:14">
-      <c r="A168" s="35"/>
-      <c r="B168" s="19"/>
-      <c r="C168" s="32"/>
-      <c r="D168" s="32"/>
-      <c r="E168" s="19"/>
-      <c r="F168" s="32"/>
-      <c r="G168" s="32"/>
-      <c r="H168" s="32"/>
-      <c r="I168" s="34"/>
-      <c r="J168" s="31"/>
-      <c r="K168" s="31"/>
-      <c r="L168" s="19"/>
-      <c r="M168" s="19"/>
-      <c r="N168" s="19"/>
-    </row>
-    <row r="169" spans="1:14">
+      <c r="L167" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M167" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N167" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" ht="16.3">
+      <c r="B168" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C168" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F168" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G168" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I168" s="34">
+        <v>298</v>
+      </c>
+      <c r="J168" s="31">
+        <v>1480000000</v>
+      </c>
+      <c r="K168" s="31">
+        <v>19000000</v>
+      </c>
+      <c r="L168" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M168" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N168" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" ht="16.3">
       <c r="A169" s="35"/>
-      <c r="B169" s="19"/>
-      <c r="C169" s="32"/>
+      <c r="B169" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C169" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="D169" s="32"/>
       <c r="E169" s="19"/>
-      <c r="F169" s="32"/>
-      <c r="G169" s="32"/>
+      <c r="F169" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G169" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H169" s="32"/>
-      <c r="I169" s="34"/>
-      <c r="J169" s="31"/>
+      <c r="I169" s="34">
+        <v>298</v>
+      </c>
+      <c r="J169" s="31">
+        <v>14.1</v>
+      </c>
       <c r="K169" s="31"/>
-      <c r="L169" s="19"/>
-      <c r="M169" s="19"/>
-      <c r="N169" s="19"/>
-    </row>
-    <row r="170" spans="1:14">
+      <c r="L169" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M169" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N169" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" ht="16.3">
       <c r="A170" s="35"/>
-      <c r="B170" s="19"/>
-      <c r="C170" s="32"/>
+      <c r="B170" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C170" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="D170" s="32"/>
       <c r="E170" s="19"/>
-      <c r="F170" s="32"/>
-      <c r="G170" s="32"/>
+      <c r="F170" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G170" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H170" s="32"/>
-      <c r="I170" s="34"/>
-      <c r="J170" s="31"/>
+      <c r="I170" s="34">
+        <v>298</v>
+      </c>
+      <c r="J170" s="31">
+        <v>5760</v>
+      </c>
       <c r="K170" s="31"/>
-      <c r="L170" s="19"/>
-      <c r="M170" s="19"/>
-      <c r="N170" s="19"/>
-    </row>
-    <row r="171" spans="1:14">
-      <c r="A171" s="35"/>
-      <c r="B171" s="19"/>
-      <c r="C171" s="32"/>
-      <c r="D171" s="32"/>
-      <c r="E171" s="19"/>
-      <c r="F171" s="32"/>
-      <c r="G171" s="32"/>
-      <c r="H171" s="32"/>
-      <c r="I171" s="34"/>
-      <c r="J171" s="31"/>
-      <c r="K171" s="31"/>
-      <c r="L171" s="19"/>
-      <c r="M171" s="19"/>
-      <c r="N171" s="19"/>
-    </row>
-    <row r="172" spans="1:14">
+      <c r="L170" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M170" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N170" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" ht="16.3">
+      <c r="B171" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C171" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F171" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G171" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I171" s="34">
+        <v>298</v>
+      </c>
+      <c r="J171" s="31">
+        <v>1251000000</v>
+      </c>
+      <c r="K171" s="31">
+        <v>2000000</v>
+      </c>
+      <c r="L171" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M171" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N171" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" ht="16.3">
       <c r="A172" s="35"/>
-      <c r="B172" s="19"/>
-      <c r="C172" s="32"/>
+      <c r="B172" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C172" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="D172" s="32"/>
       <c r="E172" s="19"/>
-      <c r="F172" s="32"/>
-      <c r="G172" s="32"/>
+      <c r="F172" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G172" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H172" s="32"/>
-      <c r="I172" s="34"/>
-      <c r="J172" s="31"/>
+      <c r="I172" s="34">
+        <v>298</v>
+      </c>
+      <c r="J172" s="31">
+        <v>7.3</v>
+      </c>
       <c r="K172" s="31"/>
-      <c r="L172" s="19"/>
-      <c r="M172" s="19"/>
-      <c r="N172" s="19"/>
-    </row>
-    <row r="173" spans="1:14">
+      <c r="L172" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M172" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N172" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" ht="16.3">
       <c r="A173" s="35"/>
-      <c r="B173" s="19"/>
-      <c r="C173" s="32"/>
+      <c r="B173" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C173" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="D173" s="32"/>
       <c r="E173" s="19"/>
-      <c r="F173" s="32"/>
-      <c r="G173" s="32"/>
+      <c r="F173" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G173" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H173" s="32"/>
-      <c r="I173" s="34"/>
-      <c r="J173" s="31"/>
+      <c r="I173" s="34">
+        <v>298</v>
+      </c>
+      <c r="J173" s="31">
+        <v>5850</v>
+      </c>
       <c r="K173" s="31"/>
-      <c r="L173" s="19"/>
-      <c r="M173" s="19"/>
-      <c r="N173" s="19"/>
-    </row>
-    <row r="174" spans="1:14">
+      <c r="L173" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M173" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N173" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" ht="16.3">
       <c r="A174" s="35"/>
-      <c r="B174" s="19"/>
-      <c r="C174" s="32"/>
-      <c r="D174" s="32"/>
-      <c r="E174" s="19"/>
-      <c r="F174" s="32"/>
-      <c r="G174" s="32"/>
-      <c r="H174" s="32"/>
-      <c r="I174" s="34"/>
-      <c r="J174" s="31"/>
-      <c r="K174" s="31"/>
-      <c r="L174" s="19"/>
-      <c r="M174" s="19"/>
-      <c r="N174" s="19"/>
-    </row>
-    <row r="175" spans="1:14">
+      <c r="B174" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C174" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F174" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G174" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I174" s="34">
+        <v>298</v>
+      </c>
+      <c r="J174" s="31">
+        <v>797000000</v>
+      </c>
+      <c r="K174" s="31">
+        <v>3000000</v>
+      </c>
+      <c r="L174" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M174" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N174" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" ht="16.3">
       <c r="A175" s="35"/>
-      <c r="B175" s="19"/>
-      <c r="C175" s="32"/>
+      <c r="B175" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C175" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="D175" s="32"/>
       <c r="E175" s="19"/>
-      <c r="F175" s="32"/>
-      <c r="G175" s="32"/>
+      <c r="F175" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G175" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H175" s="32"/>
-      <c r="I175" s="34"/>
-      <c r="J175" s="31"/>
+      <c r="I175" s="34">
+        <v>298</v>
+      </c>
+      <c r="J175" s="31">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="K175" s="31"/>
-      <c r="L175" s="19"/>
-      <c r="M175" s="19"/>
-      <c r="N175" s="19"/>
-    </row>
-    <row r="176" spans="1:14">
+      <c r="L175" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M175" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N175" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" ht="16.3">
       <c r="A176" s="35"/>
-      <c r="B176" s="19"/>
-      <c r="C176" s="32"/>
+      <c r="B176" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C176" s="32" t="s">
+        <v>64</v>
+      </c>
       <c r="D176" s="32"/>
       <c r="E176" s="19"/>
-      <c r="F176" s="32"/>
-      <c r="G176" s="32"/>
+      <c r="F176" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G176" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H176" s="32"/>
-      <c r="I176" s="34"/>
-      <c r="J176" s="31"/>
+      <c r="I176" s="34">
+        <v>298</v>
+      </c>
+      <c r="J176" s="31">
+        <v>5960</v>
+      </c>
       <c r="K176" s="31"/>
-      <c r="L176" s="19"/>
-      <c r="M176" s="19"/>
-      <c r="N176" s="19"/>
-    </row>
-    <row r="177" spans="1:14">
+      <c r="L176" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M176" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N176" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" ht="16.3">
       <c r="A177" s="35"/>
-      <c r="B177" s="19"/>
-      <c r="C177" s="32"/>
+      <c r="B177" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="C177" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D177" s="32"/>
       <c r="E177" s="19"/>
-      <c r="F177" s="32"/>
-      <c r="G177" s="32"/>
-      <c r="H177" s="32"/>
-      <c r="I177" s="34"/>
-      <c r="J177" s="31"/>
+      <c r="F177" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G177" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I177" s="34">
+        <v>298</v>
+      </c>
+      <c r="J177" s="31">
+        <v>1489000000</v>
+      </c>
       <c r="K177" s="31"/>
-      <c r="L177" s="19"/>
-      <c r="M177" s="19"/>
-      <c r="N177" s="19"/>
-    </row>
-    <row r="178" spans="1:14">
+      <c r="L177" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M177" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N177" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" ht="16.3">
       <c r="A178" s="35"/>
-      <c r="B178" s="19"/>
-      <c r="C178" s="32"/>
+      <c r="B178" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="C178" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D178" s="32"/>
       <c r="E178" s="19"/>
-      <c r="F178" s="32"/>
-      <c r="G178" s="32"/>
+      <c r="F178" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G178" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H178" s="32"/>
-      <c r="I178" s="34"/>
-      <c r="J178" s="31"/>
+      <c r="I178" s="34">
+        <v>298</v>
+      </c>
+      <c r="J178" s="31">
+        <v>21</v>
+      </c>
       <c r="K178" s="31"/>
-      <c r="L178" s="19"/>
-      <c r="M178" s="19"/>
-      <c r="N178" s="19"/>
-    </row>
-    <row r="179" spans="1:14">
+      <c r="L178" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M178" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N178" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" ht="16.3">
       <c r="A179" s="35"/>
-      <c r="B179" s="19"/>
-      <c r="C179" s="32"/>
+      <c r="B179" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="C179" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D179" s="32"/>
       <c r="E179" s="19"/>
-      <c r="F179" s="32"/>
-      <c r="G179" s="32"/>
+      <c r="F179" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G179" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H179" s="32"/>
-      <c r="I179" s="34"/>
-      <c r="J179" s="31"/>
+      <c r="I179" s="34">
+        <v>298</v>
+      </c>
+      <c r="J179" s="31">
+        <v>8900</v>
+      </c>
       <c r="K179" s="31"/>
-      <c r="L179" s="19"/>
-      <c r="M179" s="19"/>
-      <c r="N179" s="19"/>
-    </row>
-    <row r="180" spans="1:14">
+      <c r="L179" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M179" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N179" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" ht="16.3">
       <c r="A180" s="35"/>
-      <c r="B180" s="19"/>
-      <c r="C180" s="32"/>
+      <c r="B180" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C180" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D180" s="32"/>
       <c r="E180" s="19"/>
-      <c r="F180" s="32"/>
-      <c r="G180" s="32"/>
-      <c r="H180" s="32"/>
-      <c r="I180" s="34"/>
-      <c r="J180" s="31"/>
+      <c r="F180" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G180" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I180" s="34">
+        <v>298</v>
+      </c>
+      <c r="J180" s="31">
+        <v>1188000000</v>
+      </c>
       <c r="K180" s="31"/>
-      <c r="L180" s="19"/>
-      <c r="M180" s="19"/>
-      <c r="N180" s="19"/>
-    </row>
-    <row r="181" spans="1:14">
+      <c r="L180" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M180" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N180" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" ht="16.3">
       <c r="A181" s="35"/>
-      <c r="B181" s="19"/>
-      <c r="C181" s="32"/>
+      <c r="B181" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C181" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D181" s="32"/>
       <c r="E181" s="19"/>
-      <c r="F181" s="32"/>
-      <c r="G181" s="32"/>
+      <c r="F181" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G181" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H181" s="32"/>
-      <c r="I181" s="34"/>
-      <c r="J181" s="31"/>
+      <c r="I181" s="34">
+        <v>298</v>
+      </c>
+      <c r="J181" s="31">
+        <v>9.6</v>
+      </c>
       <c r="K181" s="31"/>
-      <c r="L181" s="19"/>
-      <c r="M181" s="19"/>
-      <c r="N181" s="19"/>
-    </row>
-    <row r="182" spans="1:14">
+      <c r="L181" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M181" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N181" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" ht="16.3">
       <c r="A182" s="35"/>
-      <c r="B182" s="19"/>
-      <c r="C182" s="32"/>
+      <c r="B182" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C182" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D182" s="32"/>
       <c r="E182" s="19"/>
-      <c r="F182" s="32"/>
-      <c r="G182" s="32"/>
-      <c r="H182" s="32"/>
-      <c r="I182" s="34"/>
-      <c r="J182" s="31"/>
+      <c r="F182" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G182" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I182" s="34">
+        <v>298</v>
+      </c>
+      <c r="J182" s="31">
+        <v>2350000000</v>
+      </c>
       <c r="K182" s="31"/>
-      <c r="L182" s="19"/>
-      <c r="M182" s="19"/>
-      <c r="N182" s="19"/>
-    </row>
-    <row r="183" spans="1:14">
+      <c r="L182" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M182" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N182" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="183" spans="1:14" ht="16.3">
       <c r="A183" s="35"/>
-      <c r="B183" s="19"/>
-      <c r="C183" s="32"/>
+      <c r="B183" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C183" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D183" s="32"/>
       <c r="E183" s="19"/>
-      <c r="F183" s="32"/>
-      <c r="G183" s="32"/>
+      <c r="F183" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G183" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H183" s="32"/>
-      <c r="I183" s="34"/>
-      <c r="J183" s="31"/>
+      <c r="I183" s="34">
+        <v>298</v>
+      </c>
+      <c r="J183" s="31">
+        <v>46</v>
+      </c>
       <c r="K183" s="31"/>
-      <c r="L183" s="19"/>
-      <c r="M183" s="19"/>
-      <c r="N183" s="19"/>
-    </row>
-    <row r="184" spans="1:14">
+      <c r="L183" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M183" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N183" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="184" spans="1:14" ht="16.3">
       <c r="A184" s="35"/>
-      <c r="B184" s="19"/>
-      <c r="C184" s="32"/>
+      <c r="B184" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C184" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D184" s="32"/>
       <c r="E184" s="19"/>
-      <c r="F184" s="32"/>
-      <c r="G184" s="32"/>
+      <c r="F184" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G184" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H184" s="32"/>
-      <c r="I184" s="34"/>
-      <c r="J184" s="31"/>
+      <c r="I184" s="34">
+        <v>298</v>
+      </c>
+      <c r="J184" s="31">
+        <v>9300</v>
+      </c>
       <c r="K184" s="31"/>
-      <c r="L184" s="19"/>
-      <c r="M184" s="19"/>
-      <c r="N184" s="19"/>
-    </row>
-    <row r="185" spans="1:14">
+      <c r="L184" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M184" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N184" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" ht="16.3">
       <c r="A185" s="35"/>
-      <c r="B185" s="19"/>
-      <c r="C185" s="32"/>
+      <c r="B185" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C185" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D185" s="32"/>
       <c r="E185" s="19"/>
-      <c r="F185" s="32"/>
-      <c r="G185" s="32"/>
-      <c r="H185" s="32"/>
-      <c r="I185" s="34"/>
-      <c r="J185" s="31"/>
+      <c r="F185" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G185" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I185" s="34">
+        <v>298</v>
+      </c>
+      <c r="J185" s="31">
+        <v>1415000000</v>
+      </c>
       <c r="K185" s="31"/>
-      <c r="L185" s="19"/>
-      <c r="M185" s="19"/>
-      <c r="N185" s="19"/>
-    </row>
-    <row r="186" spans="1:14">
+      <c r="L185" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M185" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N185" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" ht="16.3">
       <c r="A186" s="35"/>
-      <c r="B186" s="19"/>
-      <c r="C186" s="32"/>
+      <c r="B186" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C186" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D186" s="32"/>
       <c r="E186" s="19"/>
-      <c r="F186" s="32"/>
-      <c r="G186" s="32"/>
+      <c r="F186" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G186" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H186" s="32"/>
-      <c r="I186" s="34"/>
-      <c r="J186" s="31"/>
+      <c r="I186" s="34">
+        <v>298</v>
+      </c>
+      <c r="J186" s="31">
+        <v>30</v>
+      </c>
       <c r="K186" s="31"/>
-      <c r="L186" s="19"/>
-      <c r="M186" s="19"/>
-      <c r="N186" s="19"/>
-    </row>
-    <row r="187" spans="1:14">
+      <c r="L186" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M186" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N186" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" ht="16.3">
       <c r="A187" s="35"/>
-      <c r="B187" s="19"/>
-      <c r="C187" s="32"/>
+      <c r="B187" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C187" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D187" s="32"/>
       <c r="E187" s="19"/>
-      <c r="F187" s="32"/>
-      <c r="G187" s="32"/>
+      <c r="F187" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G187" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H187" s="32"/>
-      <c r="I187" s="34"/>
-      <c r="J187" s="31"/>
+      <c r="I187" s="34">
+        <v>298</v>
+      </c>
+      <c r="J187" s="31">
+        <v>9100</v>
+      </c>
       <c r="K187" s="31"/>
-      <c r="L187" s="19"/>
-      <c r="M187" s="19"/>
-      <c r="N187" s="19"/>
-    </row>
-    <row r="188" spans="1:14">
+      <c r="L187" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M187" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N187" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14" ht="16.3">
       <c r="A188" s="35"/>
-      <c r="B188" s="19"/>
-      <c r="C188" s="32"/>
+      <c r="B188" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C188" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D188" s="32"/>
       <c r="E188" s="19"/>
-      <c r="F188" s="32"/>
-      <c r="G188" s="32"/>
-      <c r="H188" s="32"/>
-      <c r="I188" s="34"/>
-      <c r="J188" s="31"/>
+      <c r="F188" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G188" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I188" s="34">
+        <v>298</v>
+      </c>
+      <c r="J188" s="31">
+        <v>1489000000</v>
+      </c>
       <c r="K188" s="31"/>
-      <c r="L188" s="19"/>
-      <c r="M188" s="19"/>
-      <c r="N188" s="19"/>
-    </row>
-    <row r="189" spans="1:14">
+      <c r="L188" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M188" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N188" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" ht="16.3">
       <c r="A189" s="35"/>
-      <c r="B189" s="19"/>
-      <c r="C189" s="32"/>
+      <c r="B189" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C189" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D189" s="32"/>
       <c r="E189" s="19"/>
-      <c r="F189" s="32"/>
-      <c r="G189" s="32"/>
+      <c r="F189" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G189" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H189" s="32"/>
-      <c r="I189" s="34"/>
-      <c r="J189" s="31"/>
+      <c r="I189" s="34">
+        <v>298</v>
+      </c>
+      <c r="J189" s="31">
+        <v>21</v>
+      </c>
       <c r="K189" s="31"/>
-      <c r="L189" s="19"/>
-      <c r="M189" s="19"/>
-      <c r="N189" s="19"/>
-    </row>
-    <row r="190" spans="1:14">
+      <c r="L189" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M189" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N189" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" ht="16.3">
       <c r="A190" s="35"/>
-      <c r="B190" s="19"/>
-      <c r="C190" s="32"/>
+      <c r="B190" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C190" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D190" s="32"/>
       <c r="E190" s="19"/>
-      <c r="F190" s="32"/>
-      <c r="G190" s="32"/>
+      <c r="F190" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G190" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H190" s="32"/>
-      <c r="I190" s="34"/>
-      <c r="J190" s="31"/>
+      <c r="I190" s="34">
+        <v>298</v>
+      </c>
+      <c r="J190" s="31">
+        <v>8900</v>
+      </c>
       <c r="K190" s="31"/>
-      <c r="L190" s="19"/>
-      <c r="M190" s="19"/>
-      <c r="N190" s="19"/>
-    </row>
-    <row r="191" spans="1:14">
+      <c r="L190" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M190" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N190" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" ht="16.3">
       <c r="A191" s="35"/>
-      <c r="B191" s="19"/>
-      <c r="C191" s="32"/>
+      <c r="B191" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C191" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D191" s="32"/>
       <c r="E191" s="19"/>
-      <c r="F191" s="32"/>
-      <c r="G191" s="32"/>
-      <c r="H191" s="32"/>
-      <c r="I191" s="34"/>
-      <c r="J191" s="31"/>
+      <c r="F191" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G191" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I191" s="34">
+        <v>298</v>
+      </c>
+      <c r="J191" s="31">
+        <v>1176000000</v>
+      </c>
       <c r="K191" s="31"/>
-      <c r="L191" s="19"/>
-      <c r="M191" s="19"/>
-      <c r="N191" s="19"/>
-    </row>
-    <row r="192" spans="1:14">
+      <c r="L191" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M191" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N191" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" ht="16.3">
       <c r="A192" s="35"/>
-      <c r="B192" s="19"/>
-      <c r="C192" s="32"/>
+      <c r="B192" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C192" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D192" s="32"/>
       <c r="E192" s="19"/>
-      <c r="F192" s="32"/>
-      <c r="G192" s="32"/>
+      <c r="F192" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G192" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H192" s="32"/>
-      <c r="I192" s="34"/>
-      <c r="J192" s="31"/>
+      <c r="I192" s="34">
+        <v>298</v>
+      </c>
+      <c r="J192" s="31">
+        <v>24.6</v>
+      </c>
       <c r="K192" s="31"/>
-      <c r="L192" s="19"/>
-      <c r="M192" s="19"/>
-      <c r="N192" s="19"/>
-    </row>
-    <row r="193" spans="1:14">
+      <c r="L192" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M192" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N192" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" ht="16.3">
       <c r="A193" s="35"/>
-      <c r="B193" s="19"/>
-      <c r="C193" s="32"/>
+      <c r="B193" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C193" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="D193" s="32"/>
       <c r="E193" s="19"/>
-      <c r="F193" s="32"/>
-      <c r="G193" s="32"/>
+      <c r="F193" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G193" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="H193" s="32"/>
-      <c r="I193" s="34"/>
-      <c r="J193" s="31"/>
+      <c r="I193" s="34">
+        <v>298</v>
+      </c>
+      <c r="J193" s="31">
+        <v>7900</v>
+      </c>
       <c r="K193" s="31"/>
-      <c r="L193" s="19"/>
-      <c r="M193" s="19"/>
-      <c r="N193" s="19"/>
+      <c r="L193" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="M193" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="N193" s="19" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="194" spans="1:14">
       <c r="A194" s="35"/>
@@ -11025,6 +12176,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -11039,11 +12195,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -11116,9 +12267,46 @@
     <hyperlink ref="N130" r:id="rId67" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{D3707E56-1D51-485F-85A3-BFF52FD35166}"/>
     <hyperlink ref="N131" r:id="rId68" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{CA061733-25C9-4E53-AC1C-41CCC894DAED}"/>
     <hyperlink ref="N133" r:id="rId69" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{8EE5F968-7532-47E2-A8CC-3CA851BC4AB3}"/>
+    <hyperlink ref="N134" r:id="rId70" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{5249B3BF-0D48-4A10-957F-2DAC1FABE30E}"/>
+    <hyperlink ref="N136" r:id="rId71" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{A3A01AD6-2334-494E-A515-B2683BD8002B}"/>
+    <hyperlink ref="N137" r:id="rId72" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{6D01FFA0-851E-40CE-9026-2BBF07C2E6EA}"/>
+    <hyperlink ref="N139" r:id="rId73" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{A60B14C3-BA9A-498E-A81D-069F84E2DD1A}"/>
+    <hyperlink ref="N141" r:id="rId74" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{2EBA25C4-C78B-4161-95AA-A303FFDFBA5D}"/>
+    <hyperlink ref="N143" r:id="rId75" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{86CE4D8F-0739-476F-9CE6-9D30DF33143D}"/>
+    <hyperlink ref="N145" r:id="rId76" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{4CF8A3C4-EEF6-4BEB-A022-E5550A2C93D8}"/>
+    <hyperlink ref="N147" r:id="rId77" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{B24189AC-7B6C-4313-9FCF-D37392201112}"/>
+    <hyperlink ref="N149" r:id="rId78" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{86D25217-9B5E-490F-AC28-C2AC1E890DFA}"/>
+    <hyperlink ref="N151" r:id="rId79" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{E199ACBF-F56D-49CC-B2F1-EF6220C9ABAF}"/>
+    <hyperlink ref="N153" r:id="rId80" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{B8F23B65-2CE8-40B8-A467-6C4C7A914560}"/>
+    <hyperlink ref="N154" r:id="rId81" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{28C55008-F2C1-4390-8CD4-2F8C773C5C08}"/>
+    <hyperlink ref="N156" r:id="rId82" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{BF799803-70F5-479F-B573-DE393471DA1E}"/>
+    <hyperlink ref="N157" r:id="rId83" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{49996F34-6548-46F6-81AA-B6AA5D5A22DF}"/>
+    <hyperlink ref="N159" r:id="rId84" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{8AD99ED2-107A-4C95-A9EF-8CD15ECD6EA6}"/>
+    <hyperlink ref="N160" r:id="rId85" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{0BC337B2-62E5-4720-8169-36E5440ECBF7}"/>
+    <hyperlink ref="N162" r:id="rId86" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{2C3D2B4A-F36A-43C9-AE31-EED6D0F7258F}"/>
+    <hyperlink ref="N163" r:id="rId87" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{47FC2407-3EAA-4E23-AFC9-A4408375F789}"/>
+    <hyperlink ref="N165" r:id="rId88" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{001EBAE8-E17D-4E28-A780-88E3B7369ACC}"/>
+    <hyperlink ref="N166" r:id="rId89" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{ED13FAFA-820E-43A2-9C52-94C120790E7A}"/>
+    <hyperlink ref="N168" r:id="rId90" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{76947404-35A2-483A-9FC0-7881E81FCD71}"/>
+    <hyperlink ref="N169" r:id="rId91" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{43B849CD-C732-4162-93D2-7D6EC095700A}"/>
+    <hyperlink ref="N171" r:id="rId92" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{72978B36-60E3-45B5-AF53-C4D63222E6F4}"/>
+    <hyperlink ref="N172" r:id="rId93" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{5C680370-EAD0-40C7-B33C-35859C2BE180}"/>
+    <hyperlink ref="N174" r:id="rId94" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{CFA77A49-2418-44FE-8D80-319D9E79C714}"/>
+    <hyperlink ref="N175" r:id="rId95" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{60DCEF0E-9D41-4302-81BB-70E121F492E7}"/>
+    <hyperlink ref="N177" r:id="rId96" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{21C6870E-F106-4264-819B-752E87EC8621}"/>
+    <hyperlink ref="N178" r:id="rId97" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{418418FD-8B4B-42A8-BA1E-63A798E22EFC}"/>
+    <hyperlink ref="N180" r:id="rId98" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{8A000BC9-4054-4CE4-962B-23A992565745}"/>
+    <hyperlink ref="N182" r:id="rId99" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{52040ADC-AAE3-44B6-AB76-903174A50048}"/>
+    <hyperlink ref="N183" r:id="rId100" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{FBA34C8F-142A-4A70-B7E4-0AB4B7CA9E86}"/>
+    <hyperlink ref="N185" r:id="rId101" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{2BC46676-94AF-4336-ACF5-FDF76982C81A}"/>
+    <hyperlink ref="N186" r:id="rId102" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{1F14366E-7900-4777-9D7D-5CF95E1888F8}"/>
+    <hyperlink ref="N188" r:id="rId103" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{4B44F4BA-9DC5-40D3-BDB8-164720E28B39}"/>
+    <hyperlink ref="N189" r:id="rId104" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{969FF046-F30A-41E4-9A88-4CEEE2E4E4E0}"/>
+    <hyperlink ref="N191" r:id="rId105" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{B2F87050-D518-428C-BFA8-CD635A88F898}"/>
+    <hyperlink ref="N192" r:id="rId106" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2021.159190" xr:uid="{25BE3EE0-57A2-47D3-8FF3-E003D53D27D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId70"/>
+  <pageSetup orientation="portrait" r:id="rId107"/>
 </worksheet>
 </file>
 
@@ -11127,7 +12315,7 @@
   <dimension ref="A2:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.45"/>
@@ -11142,38 +12330,41 @@
         <v>61</v>
       </c>
       <c r="B2">
-        <v>18.5</v>
+        <v>0.5</v>
       </c>
       <c r="C2">
-        <v>48</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
-        <v>18.5</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="B3">
         <f>B2/SUM(B2:J2)</f>
-        <v>0.185</v>
+        <v>0.125</v>
       </c>
       <c r="C3">
         <f>C2/SUM(B2:J2)</f>
-        <v>0.48</v>
+        <v>0.125</v>
       </c>
       <c r="D3">
         <f>D2/SUM(B2:J2)</f>
-        <v>0.185</v>
+        <v>0.25</v>
       </c>
       <c r="E3">
         <f>E2/SUM(B2:J2)</f>
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="F3">
         <f>F2/SUM(B2:J2)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G3">
         <f>G2/SUM(B2:J2)</f>
@@ -11198,23 +12389,23 @@
       </c>
       <c r="B4" s="38">
         <f>B3*100</f>
-        <v>18.5</v>
+        <v>12.5</v>
       </c>
       <c r="C4" s="38">
         <f t="shared" ref="C4:J4" si="0">C3*100</f>
-        <v>48</v>
+        <v>12.5</v>
       </c>
       <c r="D4" s="38">
         <f t="shared" si="0"/>
-        <v>18.5</v>
+        <v>25</v>
       </c>
       <c r="E4" s="38">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F4" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G4" s="38">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Revisions of October and November papers
</commit_message>
<xml_diff>
--- a/Leon_Contribution_102424.xlsx
+++ b/Leon_Contribution_102424.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Github-Codes\ULTERA-contribute-Leon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0ACFD59-4431-4F56-86AA-240E078ABEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2DB88C-8BE4-41A2-80E4-37BCF3FA089D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1667,6 +1667,33 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1716,33 +1743,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2028,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D168" sqref="D168"/>
+    <sheetView tabSelected="1" topLeftCell="E53" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63:F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.45"/>
@@ -2065,19 +2065,19 @@
       <c r="B2" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="50"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="59"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1">
@@ -2087,17 +2087,17 @@
       <c r="B3" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="52"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="61"/>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1">
@@ -2115,43 +2115,43 @@
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="66" t="s">
+      <c r="D5" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="66" t="s">
+      <c r="F5" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="66" t="s">
+      <c r="G5" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="66" t="s">
+      <c r="I5" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="66" t="s">
+      <c r="J5" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="66" t="s">
+      <c r="K5" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="66" t="s">
+      <c r="L5" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="66" t="s">
+      <c r="M5" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="66" t="s">
+      <c r="N5" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="67" t="s">
+      <c r="O5" s="49" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2162,19 +2162,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="68"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="50"/>
     </row>
     <row r="7" spans="1:20" ht="17.149999999999999" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -2219,7 +2219,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="69"/>
+      <c r="O7" s="51"/>
       <c r="P7" s="30" t="s">
         <v>40</v>
       </c>
@@ -2232,35 +2232,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60" t="s">
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="63" t="s">
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="64"/>
+      <c r="N8" s="73"/>
       <c r="O8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="70" t="s">
+      <c r="P8" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="71"/>
-      <c r="R8" s="71"/>
-      <c r="S8" s="71"/>
-      <c r="T8" s="72"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="54"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1">
       <c r="A9" s="2" t="s">
@@ -4371,7 +4371,7 @@
         <v>100</v>
       </c>
       <c r="F63" s="32" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="G63" s="40" t="s">
         <v>66</v>
@@ -4407,7 +4407,7 @@
         <v>100</v>
       </c>
       <c r="F64" s="32" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="G64" s="40" t="s">
         <v>66</v>
@@ -4444,7 +4444,7 @@
         <v>100</v>
       </c>
       <c r="F65" s="32" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="G65" s="40" t="s">
         <v>66</v>
@@ -4479,7 +4479,7 @@
         <v>100</v>
       </c>
       <c r="F66" s="32" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="G66" s="40" t="s">
         <v>66</v>
@@ -13618,11 +13618,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -13637,6 +13632,11 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -13720,7 +13720,7 @@
   <dimension ref="A2:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.45"/>
@@ -13738,42 +13738,45 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="B3">
         <f>B2/SUM(B2:J2)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.17391304347826086</v>
       </c>
       <c r="C3">
         <f>C2/SUM(B2:J2)</f>
-        <v>0.16666666666666666</v>
+        <v>0.13043478260869565</v>
       </c>
       <c r="D3">
         <f>D2/SUM(B2:J2)</f>
-        <v>0.16666666666666666</v>
+        <v>0.17391304347826086</v>
       </c>
       <c r="E3">
         <f>E2/SUM(B2:J2)</f>
-        <v>0.33333333333333331</v>
+        <v>0.17391304347826086</v>
       </c>
       <c r="F3">
         <f>F2/SUM(B2:J2)</f>
-        <v>0.25</v>
+        <v>0.17391304347826086</v>
       </c>
       <c r="G3">
         <f>G2/SUM(B2:J2)</f>
-        <v>0</v>
+        <v>0.17391304347826086</v>
       </c>
       <c r="H3">
         <f>H2/SUM(B2:J2)</f>
@@ -13794,27 +13797,27 @@
       </c>
       <c r="B4" s="38">
         <f>B3*100</f>
-        <v>8.3333333333333321</v>
+        <v>17.391304347826086</v>
       </c>
       <c r="C4" s="38">
         <f t="shared" ref="C4:J4" si="0">C3*100</f>
-        <v>16.666666666666664</v>
+        <v>13.043478260869565</v>
       </c>
       <c r="D4" s="38">
         <f t="shared" si="0"/>
-        <v>16.666666666666664</v>
+        <v>17.391304347826086</v>
       </c>
       <c r="E4" s="38">
         <f t="shared" si="0"/>
-        <v>33.333333333333329</v>
+        <v>17.391304347826086</v>
       </c>
       <c r="F4" s="38">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>17.391304347826086</v>
       </c>
       <c r="G4" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.391304347826086</v>
       </c>
       <c r="H4" s="38">
         <f t="shared" si="0"/>
@@ -13832,7 +13835,7 @@
     <row r="5" spans="1:10">
       <c r="H5" s="38">
         <f>SUM(B4:G4)</f>
-        <v>99.999999999999986</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing wrong property names
</commit_message>
<xml_diff>
--- a/Leon_Contribution_102424.xlsx
+++ b/Leon_Contribution_102424.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Github-Codes\ULTERA-contribute-Leon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73DD5C1-E12A-4FA1-85A3-1ABD4540D8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA7CEC5-6FDD-412E-BB71-6103FD1065D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1663,33 +1663,6 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1739,6 +1712,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I242" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O254" sqref="O254"/>
+    <sheetView tabSelected="1" topLeftCell="C249" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K262" sqref="K262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.45"/>
@@ -2061,19 +2061,19 @@
       <c r="B2" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="59"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="50"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1">
@@ -2083,17 +2083,17 @@
       <c r="B3" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="61"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1">
@@ -2111,43 +2111,43 @@
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="56" t="s">
+      <c r="H5" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="55" t="s">
+      <c r="K5" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="55" t="s">
+      <c r="L5" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="55" t="s">
+      <c r="M5" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="55" t="s">
+      <c r="N5" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="49" t="s">
+      <c r="O5" s="67" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2158,19 +2158,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="50"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="68"/>
     </row>
     <row r="7" spans="1:20" ht="17.149999999999999" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -2215,7 +2215,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="51"/>
+      <c r="O7" s="69"/>
       <c r="P7" s="30" t="s">
         <v>40</v>
       </c>
@@ -2228,35 +2228,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69" t="s">
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72" t="s">
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="73"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="52" t="s">
+      <c r="P8" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="53"/>
-      <c r="T8" s="54"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="72"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1">
       <c r="A9" s="2" t="s">
@@ -10117,7 +10117,7 @@
       </c>
       <c r="E223" s="19"/>
       <c r="F223" s="32" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G223" s="40" t="s">
         <v>66</v>
@@ -13614,6 +13614,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -13628,11 +13633,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>